<commit_message>
improved and cut some
</commit_message>
<xml_diff>
--- a/data/user.xlsx
+++ b/data/user.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jiaying\OneDrive\Documents\NUS\2023.2024\Sem2\DSA4213\Project\LLMasters\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39BD30EA-E460-4DC8-8429-58362CD9E0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82B9235-B53B-43D1-9E9D-8B350226296E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9288" yWindow="1704" windowWidth="13620" windowHeight="9420"/>
+    <workbookView xWindow="9132" yWindow="1392" windowWidth="13620" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="68">
   <si>
     <t>ID</t>
   </si>
@@ -56,9 +69,6 @@
   </si>
   <si>
     <t>rap</t>
-  </si>
-  <si>
-    <t>classical</t>
   </si>
   <si>
     <t>hip hop</t>
@@ -232,7 +242,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1086,12 +1096,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1147,10 +1162,10 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1161,16 +1176,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1181,16 +1196,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1201,16 +1216,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1221,10 +1236,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -1241,16 +1256,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
         <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1261,16 +1276,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1281,13 +1296,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
@@ -1301,13 +1316,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
@@ -1321,16 +1336,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1341,13 +1356,13 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -1361,16 +1376,16 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1381,16 +1396,16 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1401,13 +1416,13 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F16" t="s">
         <v>11</v>
@@ -1421,7 +1436,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
@@ -1441,16 +1456,16 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1461,16 +1476,16 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1481,13 +1496,13 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
         <v>7</v>
@@ -1501,10 +1516,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -1521,16 +1536,16 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1541,16 +1556,16 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1561,16 +1576,16 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1581,16 +1596,16 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1601,13 +1616,13 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F26" t="s">
         <v>7</v>
@@ -1621,16 +1636,16 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" t="s">
         <v>24</v>
-      </c>
-      <c r="F27" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1641,13 +1656,13 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F28" t="s">
         <v>11</v>
@@ -1661,13 +1676,13 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
@@ -1681,16 +1696,16 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D30" t="s">
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1701,16 +1716,16 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1721,16 +1736,16 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E32" t="s">
         <v>7</v>
       </c>
       <c r="F32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1741,16 +1756,16 @@
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
         <v>20</v>
-      </c>
-      <c r="F33" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1761,16 +1776,16 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1781,16 +1796,16 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" t="s">
         <v>12</v>
-      </c>
-      <c r="F35" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1801,16 +1816,16 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F36" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1821,13 +1836,13 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F37" t="s">
         <v>9</v>
@@ -1841,16 +1856,16 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E38" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" t="s">
         <v>24</v>
-      </c>
-      <c r="F38" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1861,16 +1876,16 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E39" t="s">
         <v>9</v>
       </c>
       <c r="F39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1881,16 +1896,16 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1901,16 +1916,16 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1921,16 +1936,16 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E42" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F42" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1941,13 +1956,13 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
       </c>
       <c r="E43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F43" t="s">
         <v>7</v>
@@ -1961,16 +1976,16 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D44" t="s">
         <v>9</v>
       </c>
       <c r="E44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1981,16 +1996,16 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
       </c>
       <c r="E45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2001,16 +2016,16 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
       </c>
       <c r="E46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2021,16 +2036,16 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E47" t="s">
         <v>11</v>
       </c>
       <c r="F47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -2041,7 +2056,7 @@
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D48" t="s">
         <v>9</v>
@@ -2050,7 +2065,7 @@
         <v>8</v>
       </c>
       <c r="F48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2061,13 +2076,13 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>
       </c>
       <c r="E49" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F49" t="s">
         <v>11</v>
@@ -2081,16 +2096,16 @@
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D50" t="s">
         <v>8</v>
       </c>
       <c r="E50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F50" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -2101,13 +2116,13 @@
         <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E51" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F51" t="s">
         <v>7</v>

</xml_diff>